<commit_message>
feat: add spain gp bets
</commit_message>
<xml_diff>
--- a/lib/F1_LAST_BET.xlsx
+++ b/lib/F1_LAST_BET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\BACKUP PC 27_12_2023\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80E91293-4A94-4618-A07C-A01B9F071D95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED2F3FA-DD4B-43CE-BBC2-5BF8FB3E83F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{D5F7B912-2A8C-4B04-A185-6F40DBE109E7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="58">
   <si>
     <t>Driver</t>
   </si>
@@ -195,13 +195,10 @@
     <t>SAI</t>
   </si>
   <si>
-    <t>BEA</t>
-  </si>
-  <si>
-    <t>DOO</t>
-  </si>
-  <si>
     <t>BOR</t>
+  </si>
+  <si>
+    <t>HUL</t>
   </si>
 </sst>
 </file>
@@ -261,39 +258,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -606,7 +571,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,37 +636,37 @@
         <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -709,44 +674,44 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="N3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -754,44 +719,44 @@
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="O4" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -799,44 +764,44 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -844,20 +809,20 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>43</v>
@@ -869,19 +834,19 @@
         <v>47</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>46</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -889,44 +854,44 @@
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>48</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -953,19 +918,19 @@
         <v>41</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="K8" s="1" t="s">
         <v>47</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>46</v>
@@ -979,41 +944,41 @@
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="M9" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>55</v>
@@ -1024,44 +989,44 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="O10" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1069,44 +1034,44 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>50</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1166,19 +1131,19 @@
         <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>47</v>
@@ -1190,10 +1155,10 @@
         <v>48</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>50</v>
@@ -1211,37 +1176,37 @@
         <v>40</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="L14" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1259,34 +1224,34 @@
         <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>50</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1294,41 +1259,41 @@
         <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="M16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>52</v>
@@ -1358,13 +1323,13 @@
         <v>41</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>51</v>
@@ -1373,7 +1338,7 @@
         <v>55</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>52</v>
@@ -1384,44 +1349,44 @@
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1429,11 +1394,11 @@
         <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>40</v>
@@ -1442,31 +1407,31 @@
         <v>42</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="O19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1474,26 +1439,26 @@
         <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>48</v>
@@ -1502,16 +1467,16 @@
         <v>55</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>52</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1519,7 +1484,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
@@ -1535,28 +1500,28 @@
         <v>41</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1583,25 +1548,25 @@
         <v>41</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="O22" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1609,44 +1574,44 @@
         <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="I23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O23" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1661,37 +1626,37 @@
         <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="O24" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -1706,19 +1671,19 @@
         <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>47</v>
@@ -1730,13 +1695,13 @@
         <v>51</v>
       </c>
       <c r="M25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="O25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1744,20 +1709,20 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>43</v>
@@ -1766,7 +1731,7 @@
         <v>49</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>48</v>
@@ -1775,13 +1740,13 @@
         <v>52</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -1826,7 +1791,7 @@
         <v>45</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add canada bets
</commit_message>
<xml_diff>
--- a/lib/F1_LAST_BET.xlsx
+++ b/lib/F1_LAST_BET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\BACKUP PC 27_12_2023\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED2F3FA-DD4B-43CE-BBC2-5BF8FB3E83F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005D0510-305F-49A3-83EF-9D5B55C5155E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{D5F7B912-2A8C-4B04-A185-6F40DBE109E7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="59">
   <si>
     <t>Driver</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>HUL</t>
+  </si>
+  <si>
+    <t>BEA</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,44 +677,44 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -719,44 +722,44 @@
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>48</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -764,44 +767,44 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -809,44 +812,44 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -854,14 +857,14 @@
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>42</v>
@@ -870,28 +873,28 @@
         <v>49</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>48</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -960,28 +963,28 @@
         <v>49</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="N9" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -989,17 +992,17 @@
         <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>49</v>
@@ -1017,16 +1020,16 @@
         <v>48</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="O10" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1034,17 +1037,17 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>49</v>
@@ -1059,13 +1062,13 @@
         <v>43</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>48</v>
@@ -1086,37 +1089,37 @@
         <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1124,41 +1127,41 @@
         <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>46</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>50</v>
@@ -1185,28 +1188,28 @@
         <v>49</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>43</v>
       </c>
       <c r="K14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1230,28 +1233,28 @@
         <v>42</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="L15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1266,34 +1269,34 @@
         <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>52</v>
@@ -1329,19 +1332,19 @@
         <v>47</v>
       </c>
       <c r="K17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="N17" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1356,37 +1359,37 @@
         <v>44</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>55</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1394,44 +1397,44 @@
         <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="K19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="N19" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1439,41 +1442,41 @@
         <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="M20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>45</v>
@@ -1484,44 +1487,44 @@
         <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>48</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="M21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1529,26 +1532,26 @@
         <v>34</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>47</v>
@@ -1557,13 +1560,13 @@
         <v>45</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="N22" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>48</v>
@@ -1629,13 +1632,13 @@
         <v>44</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>43</v>
@@ -1644,16 +1647,16 @@
         <v>47</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="L24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>50</v>
@@ -1674,10 +1677,10 @@
         <v>44</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>41</v>
@@ -1695,13 +1698,13 @@
         <v>51</v>
       </c>
       <c r="M25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="O25" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1716,13 +1719,13 @@
         <v>44</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>43</v>
@@ -1731,22 +1734,22 @@
         <v>49</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -1754,7 +1757,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
@@ -1767,31 +1770,31 @@
         <v>42</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="O27" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>